<commit_message>
OPTIMIZACION DE DISEÑO Y PROCESOS NO.12
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/CAMIONESFACTURA.xlsx
+++ b/ProyectoPooDist/excels/CAMIONESFACTURA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Placas</t>
   </si>
@@ -38,10 +38,10 @@
     <t>Hora de Agregado</t>
   </si>
   <si>
-    <t>YZA567</t>
-  </si>
-  <si>
-    <t>11/10/2024</t>
+    <t>VWX234</t>
+  </si>
+  <si>
+    <t>12/10/2024</t>
   </si>
   <si>
     <t>Mantenimiento</t>
@@ -50,22 +50,25 @@
     <t/>
   </si>
   <si>
-    <t>En viaje</t>
-  </si>
-  <si>
-    <t>15:11:07</t>
-  </si>
-  <si>
-    <t>VWX234</t>
-  </si>
-  <si>
-    <t>12/10/2024</t>
-  </si>
-  <si>
     <t>Funcional</t>
   </si>
   <si>
     <t>11:11:56</t>
+  </si>
+  <si>
+    <t>DEF567</t>
+  </si>
+  <si>
+    <t>25/10/2024</t>
+  </si>
+  <si>
+    <t>Combustible</t>
+  </si>
+  <si>
+    <t>FUNCIONAL</t>
+  </si>
+  <si>
+    <t>09:14:59</t>
   </si>
 </sst>
 </file>
@@ -176,22 +179,22 @@
         <v>15</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>11</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>12.0</v>
+        <v>144.0</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>11</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CAMBIOS Y ARREGLOS. RESOLUCION DEL PROBLEMA DEL ORDENAMIENTO LIMITADO AL ELIMINAR. (SE PUEDE ELIMINAR LA CANTIDAD DESEADA, Y LUEGO ACTIVAR). FUNCIONAL CIN WIFI O CON WIFI.
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/CAMIONESFACTURA.xlsx
+++ b/ProyectoPooDist/excels/CAMIONESFACTURA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Placas</t>
   </si>
@@ -78,6 +78,36 @@
   </si>
   <si>
     <t>10:47:03</t>
+  </si>
+  <si>
+    <t>ORB234</t>
+  </si>
+  <si>
+    <t>17/12/2024</t>
+  </si>
+  <si>
+    <t>03:37:34</t>
+  </si>
+  <si>
+    <t>03:38:26</t>
+  </si>
+  <si>
+    <t>No Especificado</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>03:38:55</t>
+  </si>
+  <si>
+    <t>31/12/2024</t>
+  </si>
+  <si>
+    <t>Mantenimiento</t>
+  </si>
+  <si>
+    <t>03:44:57</t>
   </si>
 </sst>
 </file>
@@ -122,7 +152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -232,6 +262,110 @@
         <v>21</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>222.0</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>